<commit_message>
add more bant spirit examples
</commit_message>
<xml_diff>
--- a/Training_set_BantSpirit/Features.xlsx
+++ b/Training_set_BantSpirit/Features.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve"> name_of_the_card</t>
   </si>
@@ -133,18 +133,6 @@
   </si>
   <si>
     <t>geist_of_saint_traft</t>
-  </si>
-  <si>
-    <t>Fetches_W</t>
-  </si>
-  <si>
-    <t>Fetches_U</t>
-  </si>
-  <si>
-    <t>Fetches_G</t>
-  </si>
-  <si>
-    <t>produces_mult</t>
   </si>
   <si>
     <t>produces_colorless</t>
@@ -489,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,16 +488,15 @@
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="6.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" customWidth="1"/>
-    <col min="10" max="12" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,52 +510,40 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
       <c r="N1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -582,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -591,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -614,20 +589,8 @@
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -644,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -653,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -673,20 +636,8 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -706,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -715,7 +666,7 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -732,20 +683,8 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -759,19 +698,19 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -791,20 +730,8 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -818,22 +745,22 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -850,20 +777,8 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -880,19 +795,19 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -909,20 +824,8 @@
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>0</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -939,19 +842,19 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -968,20 +871,8 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -995,19 +886,19 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1027,20 +918,8 @@
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1054,22 +933,22 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1086,20 +965,8 @@
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1116,13 +983,13 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -1131,10 +998,10 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -1145,20 +1012,8 @@
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1181,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1193,7 +1048,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1204,20 +1059,8 @@
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
-      <c r="R12">
-        <v>0</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1234,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1263,20 +1106,8 @@
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1296,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1322,20 +1153,8 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
-      <c r="R14">
-        <v>0</v>
-      </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1349,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1381,20 +1200,8 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1429,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -1440,20 +1247,8 @@
       <c r="O16">
         <v>0</v>
       </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>0</v>
-      </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1479,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1491,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -1499,20 +1294,8 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
-      <c r="R17">
-        <v>0</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1544,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1558,20 +1341,8 @@
       <c r="O18">
         <v>1</v>
       </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1585,19 +1356,19 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -1615,22 +1386,10 @@
         <v>1</v>
       </c>
       <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1659,37 +1418,25 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O20">
-        <v>0</v>
-      </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
-      <c r="Q20">
-        <v>0</v>
-      </c>
-      <c r="R20">
-        <v>2</v>
-      </c>
-      <c r="S20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -1715,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1724,31 +1471,19 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O21">
-        <v>0</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>2</v>
-      </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1777,37 +1512,25 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M22">
         <v>0</v>
       </c>
       <c r="N22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22">
-        <v>1</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1836,37 +1559,25 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23">
         <v>1</v>
       </c>
       <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>1</v>
-      </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="R23">
-        <v>1</v>
-      </c>
-      <c r="S23">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1892,40 +1603,28 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O24">
-        <v>0</v>
-      </c>
-      <c r="P24">
-        <v>1</v>
-      </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
-      <c r="R24">
-        <v>2</v>
-      </c>
-      <c r="S24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1951,40 +1650,28 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25">
         <v>1</v>
       </c>
       <c r="N25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="R25">
         <v>2</v>
       </c>
-      <c r="S25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2010,40 +1697,28 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>1</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
         <v>2</v>
       </c>
-      <c r="S26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2075,10 +1750,10 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -2087,18 +1762,6 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>1</v>
-      </c>
-      <c r="P27">
-        <v>3</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27">
         <v>0</v>
       </c>
     </row>

</xml_diff>